<commit_message>
updated and consolidated styles
</commit_message>
<xml_diff>
--- a/daily-status/web/app/student_activity.xlsx
+++ b/daily-status/web/app/student_activity.xlsx
@@ -6263,7 +6263,11 @@
       <c r="L3" s="2" t="n"/>
       <c r="M3" s="3" t="n"/>
       <c r="N3" s="3" t="n"/>
-      <c r="O3" s="3" t="n"/>
+      <c r="O3" s="3" t="inlineStr">
+        <is>
+          <t>D</t>
+        </is>
+      </c>
       <c r="P3" s="3" t="n"/>
       <c r="Q3" s="2" t="n"/>
       <c r="R3" s="2" t="n"/>

</xml_diff>